<commit_message>
Update the migration performance data
modified:   temp/migration_performance.xlsx
</commit_message>
<xml_diff>
--- a/haas/temp/migration_performance.xlsx
+++ b/haas/temp/migration_performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcheng8/Downloads/pci-passthrough/haas/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46300C3D-D1DF-D640-8561-0E3204F80F89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E71003-D8C7-DA46-9EE1-9BED12814F44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="17660" windowHeight="14460" xr2:uid="{FFD232B1-8150-9D40-AF18-2F9F0CACF5CF}"/>
+    <workbookView xWindow="7360" yWindow="820" windowWidth="20220" windowHeight="14360" xr2:uid="{FFD232B1-8150-9D40-AF18-2F9F0CACF5CF}"/>
   </bookViews>
   <sheets>
     <sheet name="migration_performance" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>DOWNTIME (ms)</t>
+  </si>
+  <si>
+    <t>UDP SENDER</t>
+  </si>
+  <si>
+    <t>UDP RECEIVER</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60,8 +74,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,12 +393,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9686497-C3F6-744C-B0B4-A383E44F2DA9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1.8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>